<commit_message>
assetvars completed, tape updates, data dict updates
</commit_message>
<xml_diff>
--- a/DataDictionary05092023.xlsx
+++ b/DataDictionary05092023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crmerrill/Developer/lib_python/tapestratification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crmerrill/lib/tapestratification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF8E7B7-0E72-5A4B-B90F-FEDC54240AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFB630E-BB81-AB49-B12C-1BF99483DCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{0CFC8428-1E30-8A46-AA94-E08A216C8C38}"/>
   </bookViews>
@@ -1023,9 +1023,6 @@
     <t>np.bool_</t>
   </si>
   <si>
-    <t>Consumer</t>
-  </si>
-  <si>
     <t>zip</t>
   </si>
   <si>
@@ -1410,18 +1407,6 @@
     <t/>
   </si>
   <si>
-    <t>Commercial</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CommercialAmortizing</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CommercialBullet</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CommercialRevolver</t>
-  </si>
-  <si>
     <t>CommercialABL</t>
   </si>
   <si>
@@ -1465,6 +1450,21 @@
   </si>
   <si>
     <t>Original outstanding principal balance of the loan on which interest accrues and which is due by MATDATE</t>
+  </si>
+  <si>
+    <t>ConsumerLoan</t>
+  </si>
+  <si>
+    <t>CommercialLoan</t>
+  </si>
+  <si>
+    <t>CommercialAmortizing</t>
+  </si>
+  <si>
+    <t>CommercialBullet</t>
+  </si>
+  <si>
+    <t>CommercialRevolver</t>
   </si>
 </sst>
 </file>
@@ -1899,10 +1899,10 @@
   <dimension ref="A1:W141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="84" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B104" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1962,43 +1962,43 @@
         <v>283</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>327</v>
+        <v>470</v>
       </c>
       <c r="L1" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="O1" s="16" t="s">
-        <v>335</v>
-      </c>
       <c r="P1" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>456</v>
+        <v>471</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="S1" s="16" t="s">
-        <v>457</v>
+        <v>472</v>
       </c>
       <c r="T1" s="16" t="s">
-        <v>458</v>
+        <v>473</v>
       </c>
       <c r="U1" s="16" t="s">
-        <v>459</v>
+        <v>474</v>
       </c>
       <c r="V1" s="16" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="W1" s="16" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -2015,10 +2015,10 @@
         <v>313</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="H2" t="s">
         <v>290</v>
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="W2" t="b">
         <v>1</v>
@@ -2050,10 +2050,10 @@
         <v>313</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="F3" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="H3" t="s">
         <v>291</v>
@@ -2082,10 +2082,10 @@
         <v>313</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="F4" t="s">
         <v>465</v>
-      </c>
-      <c r="F4" t="s">
-        <v>470</v>
       </c>
       <c r="H4" t="s">
         <v>291</v>
@@ -2102,7 +2102,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B5" t="s">
         <v>287</v>
@@ -2114,10 +2114,10 @@
         <v>313</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F5" t="s">
         <v>340</v>
-      </c>
-      <c r="F5" t="s">
-        <v>341</v>
       </c>
       <c r="H5" t="s">
         <v>292</v>
@@ -2146,7 +2146,7 @@
         <v>324</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="H6" t="s">
         <v>291</v>
@@ -2175,7 +2175,7 @@
         <v>324</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="H7" t="s">
         <v>290</v>
@@ -2204,10 +2204,10 @@
         <v>324</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="F8" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="H8" t="s">
         <v>290</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B9" t="s">
         <v>289</v>
@@ -2236,13 +2236,13 @@
         <v>312</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="H9" t="s">
         <v>291</v>
       </c>
       <c r="I9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B10" t="s">
         <v>289</v>
@@ -2265,13 +2265,13 @@
         <v>312</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="H10" t="s">
         <v>291</v>
       </c>
       <c r="I10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J10" t="b">
         <v>1</v>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B11" t="s">
         <v>289</v>
@@ -2294,13 +2294,13 @@
         <v>312</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="H11" t="s">
         <v>291</v>
       </c>
       <c r="I11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B12" t="s">
         <v>289</v>
@@ -2323,13 +2323,13 @@
         <v>311</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="H12" t="s">
         <v>291</v>
       </c>
       <c r="I12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J12" t="b">
         <v>1</v>
@@ -2340,7 +2340,7 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B13" t="s">
         <v>289</v>
@@ -2356,7 +2356,7 @@
         <v>291</v>
       </c>
       <c r="I13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J13" t="b">
         <v>1</v>
@@ -2367,7 +2367,7 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B14" t="s">
         <v>289</v>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B15" t="s">
         <v>289</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B16" t="s">
         <v>287</v>
@@ -2437,7 +2437,7 @@
         <v>291</v>
       </c>
       <c r="I16" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J16" t="b">
         <v>1</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B17" t="s">
         <v>287</v>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="18" spans="1:23">
       <c r="A18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B18" t="s">
         <v>287</v>
@@ -2502,7 +2502,7 @@
     </row>
     <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B19" t="s">
         <v>289</v>
@@ -2529,7 +2529,7 @@
     </row>
     <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B20" t="s">
         <v>289</v>
@@ -2545,7 +2545,7 @@
         <v>292</v>
       </c>
       <c r="I20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J20" t="b">
         <v>1</v>
@@ -2556,7 +2556,7 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B21" t="s">
         <v>289</v>
@@ -2572,7 +2572,7 @@
         <v>292</v>
       </c>
       <c r="I21" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J21" t="b">
         <v>1</v>
@@ -2599,7 +2599,7 @@
         <v>291</v>
       </c>
       <c r="I22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J22" t="b">
         <v>1</v>
@@ -2680,7 +2680,7 @@
         <v>291</v>
       </c>
       <c r="I25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J25" t="b">
         <v>1</v>
@@ -2799,7 +2799,7 @@
     </row>
     <row r="30" spans="1:23">
       <c r="A30" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B30" t="s">
         <v>289</v>
@@ -2988,7 +2988,7 @@
     </row>
     <row r="37" spans="1:23">
       <c r="A37" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B37" t="s">
         <v>289</v>
@@ -3004,7 +3004,7 @@
         <v>291</v>
       </c>
       <c r="I37" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J37" t="b">
         <v>1</v>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="38" spans="1:23">
       <c r="A38" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B38" t="s">
         <v>289</v>
@@ -3024,7 +3024,7 @@
         <v>321</v>
       </c>
       <c r="D38" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E38" s="2"/>
       <c r="H38" t="s">
@@ -3042,7 +3042,7 @@
     </row>
     <row r="39" spans="1:23">
       <c r="A39" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B39" t="s">
         <v>289</v>
@@ -3058,7 +3058,7 @@
         <v>292</v>
       </c>
       <c r="I39" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J39" t="b">
         <v>1</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="40" spans="1:23">
       <c r="A40" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B40" t="s">
         <v>289</v>
@@ -3085,7 +3085,7 @@
         <v>292</v>
       </c>
       <c r="I40" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J40" t="b">
         <v>1</v>
@@ -3096,7 +3096,7 @@
     </row>
     <row r="41" spans="1:23">
       <c r="A41" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B41" t="s">
         <v>287</v>
@@ -3123,7 +3123,7 @@
     </row>
     <row r="42" spans="1:23">
       <c r="A42" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B42" t="s">
         <v>288</v>
@@ -3132,7 +3132,7 @@
         <v>321</v>
       </c>
       <c r="D42" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E42" s="2"/>
       <c r="H42" t="s">
@@ -3150,7 +3150,7 @@
     </row>
     <row r="43" spans="1:23">
       <c r="A43" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B43" t="s">
         <v>288</v>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="44" spans="1:23">
       <c r="A44" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B44" t="s">
         <v>288</v>
@@ -3186,7 +3186,7 @@
         <v>321</v>
       </c>
       <c r="D44" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E44" s="2"/>
       <c r="H44" t="s">
@@ -3204,7 +3204,7 @@
     </row>
     <row r="45" spans="1:23">
       <c r="A45" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B45" t="s">
         <v>289</v>
@@ -3231,7 +3231,7 @@
     </row>
     <row r="46" spans="1:23">
       <c r="A46" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B46" t="s">
         <v>288</v>
@@ -3258,7 +3258,7 @@
     </row>
     <row r="47" spans="1:23">
       <c r="A47" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B47" t="s">
         <v>288</v>
@@ -3285,7 +3285,7 @@
     </row>
     <row r="48" spans="1:23">
       <c r="A48" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B48" t="s">
         <v>288</v>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="49" spans="1:23">
       <c r="A49" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B49" t="s">
         <v>287</v>
@@ -3341,7 +3341,7 @@
     </row>
     <row r="50" spans="1:23">
       <c r="A50" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B50" t="s">
         <v>289</v>
@@ -3368,7 +3368,7 @@
     </row>
     <row r="51" spans="1:23">
       <c r="A51" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B51" t="s">
         <v>289</v>
@@ -3479,7 +3479,7 @@
         <v>281</v>
       </c>
       <c r="B55" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C55" t="s">
         <v>322</v>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H55" t="s">
         <v>290</v>
@@ -3506,10 +3506,10 @@
     </row>
     <row r="56" spans="1:23">
       <c r="A56" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B56" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C56" t="s">
         <v>322</v>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H56" t="s">
         <v>290</v>
@@ -3536,10 +3536,10 @@
     </row>
     <row r="57" spans="1:23">
       <c r="A57" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B57" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C57" t="s">
         <v>322</v>
@@ -3549,7 +3549,7 @@
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H57" t="s">
         <v>290</v>
@@ -3566,10 +3566,10 @@
     </row>
     <row r="58" spans="1:23">
       <c r="A58" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B58" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C58" t="s">
         <v>315</v>
@@ -3593,10 +3593,10 @@
     </row>
     <row r="59" spans="1:23">
       <c r="A59" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B59" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C59" t="s">
         <v>315</v>
@@ -3620,7 +3620,7 @@
     </row>
     <row r="60" spans="1:23">
       <c r="A60" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B60" t="s">
         <v>289</v>
@@ -3636,7 +3636,7 @@
         <v>292</v>
       </c>
       <c r="I60" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J60" t="b">
         <v>0</v>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="61" spans="1:23">
       <c r="A61" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B61" t="s">
         <v>289</v>
@@ -3674,7 +3674,7 @@
     </row>
     <row r="62" spans="1:23">
       <c r="A62" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B62" t="s">
         <v>289</v>
@@ -3690,7 +3690,7 @@
         <v>292</v>
       </c>
       <c r="I62" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J62" t="b">
         <v>0</v>
@@ -3701,7 +3701,7 @@
     </row>
     <row r="63" spans="1:23">
       <c r="A63" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B63" t="s">
         <v>288</v>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="64" spans="1:23">
       <c r="A64" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B64" t="s">
         <v>289</v>
@@ -3755,7 +3755,7 @@
     </row>
     <row r="65" spans="1:16">
       <c r="A65" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B65" t="s">
         <v>288</v>
@@ -3809,7 +3809,7 @@
     </row>
     <row r="67" spans="1:16">
       <c r="A67" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B67" t="s">
         <v>323</v>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="68" spans="1:16">
       <c r="A68" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B68" t="s">
         <v>323</v>
@@ -3863,7 +3863,7 @@
     </row>
     <row r="69" spans="1:16">
       <c r="A69" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B69" t="s">
         <v>323</v>
@@ -3890,7 +3890,7 @@
     </row>
     <row r="70" spans="1:16">
       <c r="A70" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B70" t="s">
         <v>323</v>
@@ -3902,10 +3902,10 @@
         <v>313</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F70" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="H70" t="s">
         <v>291</v>
@@ -3922,7 +3922,7 @@
     </row>
     <row r="71" spans="1:16">
       <c r="A71" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B71" t="s">
         <v>287</v>
@@ -3949,7 +3949,7 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B72" t="s">
         <v>289</v>
@@ -3961,13 +3961,13 @@
         <v>311</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H72" t="s">
         <v>292</v>
       </c>
       <c r="I72" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J72" t="b">
         <v>0</v>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="73" spans="1:16">
       <c r="A73" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B73" t="s">
         <v>289</v>
@@ -4006,7 +4006,7 @@
         <v>292</v>
       </c>
       <c r="I73" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J73" t="b">
         <v>0</v>
@@ -4017,7 +4017,7 @@
     </row>
     <row r="74" spans="1:16">
       <c r="A74" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B74" t="s">
         <v>289</v>
@@ -4033,7 +4033,7 @@
         <v>292</v>
       </c>
       <c r="I74" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J74" t="b">
         <v>0</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="75" spans="1:16">
       <c r="A75" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B75" t="s">
         <v>289</v>
@@ -4056,13 +4056,13 @@
         <v>311</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H75" t="s">
         <v>292</v>
       </c>
       <c r="I75" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J75" t="b">
         <v>0</v>
@@ -4085,7 +4085,7 @@
     </row>
     <row r="76" spans="1:16">
       <c r="A76" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B76" t="s">
         <v>289</v>
@@ -4101,7 +4101,7 @@
         <v>292</v>
       </c>
       <c r="I76" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J76" t="b">
         <v>0</v>
@@ -4112,7 +4112,7 @@
     </row>
     <row r="77" spans="1:16">
       <c r="A77" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B77" t="s">
         <v>289</v>
@@ -4128,7 +4128,7 @@
         <v>292</v>
       </c>
       <c r="I77" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J77" t="b">
         <v>0</v>
@@ -4142,7 +4142,7 @@
         <v>284</v>
       </c>
       <c r="B78" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C78" t="s">
         <v>314</v>
@@ -4151,7 +4151,7 @@
         <v>313</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H78" t="s">
         <v>290</v>
@@ -4180,7 +4180,7 @@
     </row>
     <row r="79" spans="1:16">
       <c r="A79" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B79" t="s">
         <v>289</v>
@@ -4192,7 +4192,7 @@
         <v>311</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H79" t="s">
         <v>290</v>
@@ -4233,7 +4233,7 @@
         <v>313</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H80" t="s">
         <v>290</v>
@@ -4262,7 +4262,7 @@
     </row>
     <row r="81" spans="1:16">
       <c r="A81" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B81" t="s">
         <v>289</v>
@@ -4278,7 +4278,7 @@
         <v>292</v>
       </c>
       <c r="I81" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J81" t="b">
         <v>0</v>
@@ -4301,7 +4301,7 @@
     </row>
     <row r="82" spans="1:16">
       <c r="A82" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B82" t="s">
         <v>289</v>
@@ -4313,7 +4313,7 @@
         <v>311</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H82" t="s">
         <v>290</v>
@@ -4330,7 +4330,7 @@
     </row>
     <row r="83" spans="1:16">
       <c r="A83" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B83" t="s">
         <v>289</v>
@@ -4353,7 +4353,7 @@
     </row>
     <row r="84" spans="1:16">
       <c r="A84" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B84" t="s">
         <v>289</v>
@@ -4376,7 +4376,7 @@
     </row>
     <row r="85" spans="1:16">
       <c r="A85" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B85" t="s">
         <v>289</v>
@@ -4399,7 +4399,7 @@
     </row>
     <row r="86" spans="1:16">
       <c r="A86" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B86" t="s">
         <v>289</v>
@@ -4422,7 +4422,7 @@
     </row>
     <row r="87" spans="1:16">
       <c r="A87" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B87" t="s">
         <v>289</v>
@@ -4445,7 +4445,7 @@
     </row>
     <row r="88" spans="1:16">
       <c r="A88" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B88" t="s">
         <v>289</v>
@@ -4468,7 +4468,7 @@
     </row>
     <row r="89" spans="1:16">
       <c r="A89" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B89" t="s">
         <v>289</v>
@@ -4491,7 +4491,7 @@
     </row>
     <row r="90" spans="1:16">
       <c r="A90" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B90" t="s">
         <v>289</v>
@@ -4514,7 +4514,7 @@
     </row>
     <row r="91" spans="1:16">
       <c r="A91" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B91" t="s">
         <v>289</v>
@@ -4537,7 +4537,7 @@
     </row>
     <row r="92" spans="1:16">
       <c r="A92" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B92" t="s">
         <v>289</v>
@@ -4560,7 +4560,7 @@
     </row>
     <row r="93" spans="1:16">
       <c r="A93" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B93" t="s">
         <v>289</v>
@@ -4583,7 +4583,7 @@
     </row>
     <row r="94" spans="1:16">
       <c r="A94" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B94" t="s">
         <v>289</v>
@@ -4592,7 +4592,7 @@
         <v>321</v>
       </c>
       <c r="D94" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="H94" t="s">
         <v>290</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="95" spans="1:16">
       <c r="A95" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B95" t="s">
         <v>288</v>
@@ -4615,7 +4615,7 @@
         <v>321</v>
       </c>
       <c r="D95" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="H95" t="s">
         <v>290</v>
@@ -4629,7 +4629,7 @@
     </row>
     <row r="96" spans="1:16">
       <c r="A96" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B96" t="s">
         <v>287</v>
@@ -4653,7 +4653,7 @@
     </row>
     <row r="97" spans="1:21">
       <c r="A97" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B97" t="s">
         <v>287</v>
@@ -4677,7 +4677,7 @@
     </row>
     <row r="98" spans="1:21">
       <c r="A98" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B98" t="s">
         <v>289</v>
@@ -4701,7 +4701,7 @@
     </row>
     <row r="99" spans="1:21">
       <c r="A99" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B99" t="s">
         <v>289</v>
@@ -4725,7 +4725,7 @@
     </row>
     <row r="100" spans="1:21">
       <c r="A100" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B100" t="s">
         <v>289</v>
@@ -4752,7 +4752,7 @@
     </row>
     <row r="101" spans="1:21">
       <c r="A101" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B101" t="s">
         <v>289</v>
@@ -4776,7 +4776,7 @@
     </row>
     <row r="102" spans="1:21">
       <c r="A102" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B102" t="s">
         <v>287</v>
@@ -4800,7 +4800,7 @@
     </row>
     <row r="103" spans="1:21">
       <c r="A103" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B103" t="s">
         <v>289</v>
@@ -4824,7 +4824,7 @@
     </row>
     <row r="104" spans="1:21">
       <c r="A104" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B104" t="s">
         <v>287</v>
@@ -4848,7 +4848,7 @@
     </row>
     <row r="105" spans="1:21">
       <c r="A105" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B105" t="s">
         <v>287</v>
@@ -4872,7 +4872,7 @@
     </row>
     <row r="106" spans="1:21">
       <c r="A106" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B106" t="s">
         <v>289</v>
@@ -4896,7 +4896,7 @@
     </row>
     <row r="107" spans="1:21">
       <c r="A107" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B107" t="s">
         <v>289</v>
@@ -4920,7 +4920,7 @@
     </row>
     <row r="108" spans="1:21">
       <c r="A108" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B108" t="s">
         <v>289</v>
@@ -4944,7 +4944,7 @@
     </row>
     <row r="109" spans="1:21">
       <c r="A109" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B109" t="s">
         <v>320</v>
@@ -4971,7 +4971,7 @@
     </row>
     <row r="110" spans="1:21">
       <c r="A110" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B110" t="s">
         <v>287</v>
@@ -5023,7 +5023,7 @@
     </row>
     <row r="112" spans="1:21">
       <c r="A112" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B112" t="s">
         <v>288</v>
@@ -5049,7 +5049,7 @@
     </row>
     <row r="113" spans="1:16">
       <c r="A113" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B113" t="s">
         <v>288</v>
@@ -5127,7 +5127,7 @@
     </row>
     <row r="116" spans="1:16">
       <c r="A116" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B116" t="s">
         <v>288</v>
@@ -5153,7 +5153,7 @@
     </row>
     <row r="117" spans="1:16">
       <c r="A117" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B117" t="s">
         <v>289</v>
@@ -5179,7 +5179,7 @@
     </row>
     <row r="118" spans="1:16">
       <c r="A118" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B118" t="s">
         <v>288</v>
@@ -5240,7 +5240,7 @@
     </row>
     <row r="120" spans="1:16">
       <c r="A120" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B120" t="s">
         <v>289</v>
@@ -5275,7 +5275,7 @@
     </row>
     <row r="121" spans="1:16">
       <c r="A121" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B121" t="s">
         <v>287</v>
@@ -5310,10 +5310,10 @@
     </row>
     <row r="122" spans="1:16">
       <c r="A122" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B122" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C122" t="s">
         <v>322</v>
@@ -5342,7 +5342,7 @@
     </row>
     <row r="123" spans="1:16">
       <c r="A123" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B123" t="s">
         <v>289</v>
@@ -5362,7 +5362,7 @@
     </row>
     <row r="124" spans="1:16">
       <c r="A124" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B124" t="s">
         <v>289</v>
@@ -5382,7 +5382,7 @@
     </row>
     <row r="125" spans="1:16">
       <c r="A125" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B125" t="s">
         <v>287</v>
@@ -5414,7 +5414,7 @@
         <v>311</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H126" t="s">
         <v>292</v>
@@ -5452,7 +5452,7 @@
         <v>313</v>
       </c>
       <c r="E127" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H127" t="s">
         <v>290</v>
@@ -5493,7 +5493,7 @@
         <v>313</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H128" t="s">
         <v>290</v>
@@ -5598,7 +5598,7 @@
     </row>
     <row r="131" spans="1:16">
       <c r="A131" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B131" t="s">
         <v>287</v>
@@ -5636,7 +5636,7 @@
     </row>
     <row r="132" spans="1:16">
       <c r="A132" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B132" t="s">
         <v>287</v>
@@ -5674,7 +5674,7 @@
     </row>
     <row r="133" spans="1:16">
       <c r="A133" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B133" t="s">
         <v>289</v>
@@ -5709,7 +5709,7 @@
     </row>
     <row r="134" spans="1:16">
       <c r="A134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B134" t="s">
         <v>289</v>
@@ -5732,7 +5732,7 @@
     </row>
     <row r="135" spans="1:16">
       <c r="A135" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B135" t="s">
         <v>288</v>
@@ -5755,7 +5755,7 @@
     </row>
     <row r="136" spans="1:16">
       <c r="A136" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B136" t="s">
         <v>287</v>
@@ -5778,7 +5778,7 @@
     </row>
     <row r="137" spans="1:16">
       <c r="A137" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B137" t="s">
         <v>287</v>
@@ -5801,7 +5801,7 @@
     </row>
     <row r="138" spans="1:16">
       <c r="A138" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B138" t="s">
         <v>288</v>
@@ -5848,7 +5848,7 @@
     </row>
     <row r="140" spans="1:16">
       <c r="A140" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B140" t="s">
         <v>287</v>

</xml_diff>

<commit_message>
tape completed, assetvars completed, strattool updates, datadict almost complete
</commit_message>
<xml_diff>
--- a/DataDictionary05092023.xlsx
+++ b/DataDictionary05092023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crmerrill/Developer/lib_python/tapestratification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crmerrill/lib/tapestratification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD2935C-151B-5B48-8FC0-ABC509114FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B246711-7600-B549-941B-D2B2BF0A78F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{0CFC8428-1E30-8A46-AA94-E08A216C8C38}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="47500" windowHeight="23940" xr2:uid="{0CFC8428-1E30-8A46-AA94-E08A216C8C38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$X$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$X$150</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$I$91</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="510">
   <si>
     <t>loanid</t>
   </si>
@@ -1555,6 +1555,21 @@
   </si>
   <si>
     <t>Sub-category specific to prop_category (ex. Prop_category = auto_retail ; prop_category2 = sedan)</t>
+  </si>
+  <si>
+    <t>svc_sub_name</t>
+  </si>
+  <si>
+    <t>svc_sub_fee_type</t>
+  </si>
+  <si>
+    <t>svc_sub_fee_gross</t>
+  </si>
+  <si>
+    <t>svc_sub_fee2_type</t>
+  </si>
+  <si>
+    <t>svc_sub_fee2_gross</t>
   </si>
 </sst>
 </file>
@@ -1993,13 +2008,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434BD60A-FB0C-6840-A282-2A366498F430}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:X145"/>
+  <dimension ref="A1:X150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B109" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A109" sqref="A109"/>
+      <selection pane="bottomRight" activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7022,8 +7037,8 @@
       </c>
     </row>
     <row r="110" spans="1:23">
-      <c r="A110" t="s">
-        <v>341</v>
+      <c r="A110" s="17" t="s">
+        <v>505</v>
       </c>
       <c r="B110" t="s">
         <v>287</v>
@@ -7034,239 +7049,91 @@
       <c r="D110" t="s">
         <v>313</v>
       </c>
-      <c r="H110" t="s">
-        <v>291</v>
-      </c>
-      <c r="K110" t="b">
-        <v>0</v>
-      </c>
-      <c r="L110" t="b">
-        <v>1</v>
-      </c>
-      <c r="M110" t="b">
-        <v>1</v>
-      </c>
-      <c r="R110" t="b">
-        <v>0</v>
-      </c>
-      <c r="S110" t="b">
-        <v>0</v>
-      </c>
-      <c r="T110" t="b">
-        <v>0</v>
-      </c>
-      <c r="U110" t="b">
-        <v>0</v>
-      </c>
-      <c r="V110" t="b">
-        <v>0</v>
-      </c>
-      <c r="W110" t="b">
-        <v>0</v>
-      </c>
+      <c r="E110" s="3"/>
     </row>
     <row r="111" spans="1:23">
-      <c r="A111" t="s">
-        <v>298</v>
+      <c r="A111" s="17" t="s">
+        <v>506</v>
       </c>
       <c r="B111" t="s">
         <v>287</v>
       </c>
       <c r="C111" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D111" t="s">
-        <v>312</v>
-      </c>
-      <c r="H111" t="s">
-        <v>292</v>
-      </c>
-      <c r="K111" t="b">
-        <v>0</v>
-      </c>
-      <c r="L111" t="b">
-        <v>1</v>
-      </c>
-      <c r="M111" t="b">
-        <v>1</v>
-      </c>
-      <c r="R111" t="b">
-        <v>0</v>
-      </c>
-      <c r="S111" t="b">
-        <v>0</v>
-      </c>
-      <c r="T111" t="b">
-        <v>0</v>
-      </c>
-      <c r="U111" t="b">
-        <v>0</v>
-      </c>
-      <c r="V111" t="b">
-        <v>0</v>
-      </c>
-      <c r="W111" t="b">
-        <v>0</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="E111" s="3"/>
     </row>
     <row r="112" spans="1:23">
-      <c r="A112" t="s">
-        <v>345</v>
+      <c r="A112" s="17" t="s">
+        <v>507</v>
       </c>
       <c r="B112" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C112" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="D112" t="s">
-        <v>324</v>
-      </c>
-      <c r="E112" t="s">
-        <v>472</v>
-      </c>
-      <c r="H112" t="s">
-        <v>290</v>
-      </c>
-      <c r="K112" t="b">
-        <v>0</v>
-      </c>
-      <c r="L112" t="b">
-        <v>1</v>
-      </c>
-      <c r="M112" t="b">
-        <v>1</v>
-      </c>
-      <c r="R112" t="b">
-        <v>0</v>
-      </c>
-      <c r="S112" t="b">
-        <v>0</v>
-      </c>
-      <c r="T112" t="b">
-        <v>0</v>
-      </c>
-      <c r="U112" t="b">
-        <v>0</v>
-      </c>
-      <c r="V112" t="b">
-        <v>0</v>
-      </c>
-      <c r="W112" t="b">
-        <v>0</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="E112" s="3"/>
     </row>
     <row r="113" spans="1:23">
-      <c r="A113" t="s">
-        <v>344</v>
+      <c r="A113" s="17" t="s">
+        <v>508</v>
       </c>
       <c r="B113" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C113" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D113" t="s">
-        <v>324</v>
-      </c>
-      <c r="H113" t="s">
-        <v>290</v>
-      </c>
-      <c r="K113" t="b">
-        <v>0</v>
-      </c>
-      <c r="L113" t="b">
-        <v>1</v>
-      </c>
-      <c r="M113" t="b">
-        <v>1</v>
-      </c>
-      <c r="R113" t="b">
-        <v>0</v>
-      </c>
-      <c r="S113" t="b">
-        <v>0</v>
-      </c>
-      <c r="T113" t="b">
-        <v>0</v>
-      </c>
-      <c r="U113" t="b">
-        <v>0</v>
-      </c>
-      <c r="V113" t="b">
-        <v>0</v>
-      </c>
-      <c r="W113" t="b">
-        <v>0</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="E113" s="3"/>
     </row>
     <row r="114" spans="1:23">
-      <c r="A114" t="s">
-        <v>299</v>
+      <c r="A114" s="17" t="s">
+        <v>509</v>
       </c>
       <c r="B114" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C114" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D114" t="s">
-        <v>313</v>
-      </c>
-      <c r="H114" t="s">
-        <v>291</v>
-      </c>
-      <c r="K114" t="b">
-        <v>0</v>
-      </c>
-      <c r="M114" t="b">
-        <v>1</v>
-      </c>
-      <c r="N114" t="b">
-        <v>1</v>
-      </c>
-      <c r="R114" t="b">
-        <v>0</v>
-      </c>
-      <c r="S114" t="b">
-        <v>0</v>
-      </c>
-      <c r="T114" t="b">
-        <v>0</v>
-      </c>
-      <c r="U114" t="b">
-        <v>0</v>
-      </c>
-      <c r="V114" t="b">
-        <v>0</v>
-      </c>
-      <c r="W114" t="b">
-        <v>0</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="E114" s="3"/>
     </row>
     <row r="115" spans="1:23">
       <c r="A115" t="s">
-        <v>300</v>
+        <v>341</v>
       </c>
       <c r="B115" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C115" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D115" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="H115" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="K115" t="b">
         <v>0</v>
       </c>
+      <c r="L115" t="b">
+        <v>1</v>
+      </c>
       <c r="M115" t="b">
-        <v>1</v>
-      </c>
-      <c r="N115" t="b">
         <v>1</v>
       </c>
       <c r="R115" t="b">
@@ -7290,33 +7157,27 @@
     </row>
     <row r="116" spans="1:23">
       <c r="A116" t="s">
-        <v>395</v>
+        <v>298</v>
       </c>
       <c r="B116" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C116" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D116" t="s">
-        <v>324</v>
-      </c>
-      <c r="E116" t="s">
-        <v>470</v>
-      </c>
-      <c r="F116" t="s">
-        <v>471</v>
+        <v>312</v>
       </c>
       <c r="H116" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="K116" t="b">
         <v>0</v>
       </c>
+      <c r="L116" t="b">
+        <v>1</v>
+      </c>
       <c r="M116" t="b">
-        <v>1</v>
-      </c>
-      <c r="N116" t="b">
         <v>1</v>
       </c>
       <c r="R116" t="b">
@@ -7340,16 +7201,19 @@
     </row>
     <row r="117" spans="1:23">
       <c r="A117" t="s">
-        <v>396</v>
+        <v>345</v>
       </c>
       <c r="B117" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C117" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D117" t="s">
-        <v>311</v>
+        <v>324</v>
+      </c>
+      <c r="E117" t="s">
+        <v>472</v>
       </c>
       <c r="H117" t="s">
         <v>290</v>
@@ -7384,7 +7248,7 @@
     </row>
     <row r="118" spans="1:23">
       <c r="A118" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B118" t="s">
         <v>288</v>
@@ -7428,7 +7292,7 @@
     </row>
     <row r="119" spans="1:23">
       <c r="A119" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B119" t="s">
         <v>287</v>
@@ -7449,16 +7313,7 @@
         <v>1</v>
       </c>
       <c r="N119" t="b">
-        <v>0</v>
-      </c>
-      <c r="O119" t="b">
-        <v>0</v>
-      </c>
-      <c r="P119" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q119" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R119" t="b">
         <v>0</v>
@@ -7481,19 +7336,19 @@
     </row>
     <row r="120" spans="1:23">
       <c r="A120" t="s">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="B120" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C120" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D120" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="H120" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K120" t="b">
         <v>0</v>
@@ -7502,16 +7357,7 @@
         <v>1</v>
       </c>
       <c r="N120" t="b">
-        <v>0</v>
-      </c>
-      <c r="O120" t="b">
-        <v>0</v>
-      </c>
-      <c r="P120" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R120" t="b">
         <v>0</v>
@@ -7534,19 +7380,25 @@
     </row>
     <row r="121" spans="1:23">
       <c r="A121" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B121" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C121" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D121" t="s">
-        <v>313</v>
+        <v>324</v>
+      </c>
+      <c r="E121" t="s">
+        <v>470</v>
+      </c>
+      <c r="F121" t="s">
+        <v>471</v>
       </c>
       <c r="H121" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K121" t="b">
         <v>0</v>
@@ -7555,16 +7407,7 @@
         <v>1</v>
       </c>
       <c r="N121" t="b">
-        <v>0</v>
-      </c>
-      <c r="O121" t="b">
-        <v>0</v>
-      </c>
-      <c r="P121" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q121" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R121" t="b">
         <v>0</v>
@@ -7587,37 +7430,28 @@
     </row>
     <row r="122" spans="1:23">
       <c r="A122" t="s">
-        <v>361</v>
+        <v>396</v>
       </c>
       <c r="B122" t="s">
-        <v>374</v>
+        <v>289</v>
       </c>
       <c r="C122" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D122" t="s">
-        <v>467</v>
-      </c>
-      <c r="F122" s="11" t="s">
-        <v>493</v>
+        <v>311</v>
+      </c>
+      <c r="H122" t="s">
+        <v>290</v>
       </c>
       <c r="K122" t="b">
         <v>0</v>
       </c>
+      <c r="L122" t="b">
+        <v>1</v>
+      </c>
       <c r="M122" t="b">
         <v>1</v>
-      </c>
-      <c r="N122" t="b">
-        <v>0</v>
-      </c>
-      <c r="O122" t="b">
-        <v>0</v>
-      </c>
-      <c r="P122" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q122" t="b">
-        <v>0</v>
       </c>
       <c r="R122" t="b">
         <v>0</v>
@@ -7640,19 +7474,25 @@
     </row>
     <row r="123" spans="1:23">
       <c r="A123" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="B123" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C123" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D123" t="s">
-        <v>311</v>
+        <v>324</v>
+      </c>
+      <c r="H123" t="s">
+        <v>290</v>
       </c>
       <c r="K123" t="b">
         <v>0</v>
+      </c>
+      <c r="L123" t="b">
+        <v>1</v>
       </c>
       <c r="M123" t="b">
         <v>1</v>
@@ -7678,22 +7518,37 @@
     </row>
     <row r="124" spans="1:23">
       <c r="A124" t="s">
-        <v>363</v>
+        <v>301</v>
       </c>
       <c r="B124" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C124" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D124" t="s">
-        <v>311</v>
+        <v>313</v>
+      </c>
+      <c r="H124" t="s">
+        <v>291</v>
       </c>
       <c r="K124" t="b">
         <v>0</v>
       </c>
       <c r="M124" t="b">
         <v>1</v>
+      </c>
+      <c r="N124" t="b">
+        <v>0</v>
+      </c>
+      <c r="O124" t="b">
+        <v>0</v>
+      </c>
+      <c r="P124" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q124" t="b">
+        <v>0</v>
       </c>
       <c r="R124" t="b">
         <v>0</v>
@@ -7716,22 +7571,37 @@
     </row>
     <row r="125" spans="1:23">
       <c r="A125" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B125" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C125" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D125" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+      <c r="H125" t="s">
+        <v>292</v>
       </c>
       <c r="K125" t="b">
         <v>0</v>
       </c>
       <c r="M125" t="b">
         <v>1</v>
+      </c>
+      <c r="N125" t="b">
+        <v>0</v>
+      </c>
+      <c r="O125" t="b">
+        <v>0</v>
+      </c>
+      <c r="P125" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q125" t="b">
+        <v>0</v>
       </c>
       <c r="R125" t="b">
         <v>0</v>
@@ -7754,19 +7624,16 @@
     </row>
     <row r="126" spans="1:23">
       <c r="A126" t="s">
-        <v>296</v>
+        <v>397</v>
       </c>
       <c r="B126" t="s">
-        <v>320</v>
+        <v>287</v>
       </c>
       <c r="C126" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D126" t="s">
-        <v>311</v>
-      </c>
-      <c r="E126" t="s">
-        <v>489</v>
+        <v>313</v>
       </c>
       <c r="H126" t="s">
         <v>292</v>
@@ -7778,7 +7645,7 @@
         <v>1</v>
       </c>
       <c r="N126" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O126" t="b">
         <v>0</v>
@@ -7810,22 +7677,19 @@
     </row>
     <row r="127" spans="1:23">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>361</v>
       </c>
       <c r="B127" t="s">
-        <v>287</v>
+        <v>374</v>
       </c>
       <c r="C127" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="D127" t="s">
-        <v>313</v>
-      </c>
-      <c r="E127" t="s">
-        <v>490</v>
-      </c>
-      <c r="F127" t="s">
-        <v>491</v>
+        <v>467</v>
+      </c>
+      <c r="F127" s="11" t="s">
+        <v>493</v>
       </c>
       <c r="K127" t="b">
         <v>0</v>
@@ -7834,7 +7698,7 @@
         <v>1</v>
       </c>
       <c r="N127" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O127" t="b">
         <v>0</v>
@@ -7866,46 +7730,22 @@
     </row>
     <row r="128" spans="1:23">
       <c r="A128" t="s">
-        <v>130</v>
+        <v>362</v>
       </c>
       <c r="B128" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C128" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D128" t="s">
-        <v>313</v>
-      </c>
-      <c r="E128" t="s">
-        <v>347</v>
-      </c>
-      <c r="F128" t="s">
-        <v>491</v>
-      </c>
-      <c r="H128" t="s">
-        <v>290</v>
-      </c>
-      <c r="I128" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="K128" t="b">
         <v>0</v>
       </c>
       <c r="M128" t="b">
         <v>1</v>
-      </c>
-      <c r="N128" t="b">
-        <v>1</v>
-      </c>
-      <c r="O128" t="b">
-        <v>0</v>
-      </c>
-      <c r="P128" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q128" t="b">
-        <v>0</v>
       </c>
       <c r="R128" t="b">
         <v>0</v>
@@ -7928,43 +7768,22 @@
     </row>
     <row r="129" spans="1:23">
       <c r="A129" t="s">
-        <v>297</v>
+        <v>363</v>
       </c>
       <c r="B129" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C129" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D129" t="s">
-        <v>313</v>
-      </c>
-      <c r="E129" t="s">
-        <v>492</v>
-      </c>
-      <c r="H129" t="s">
-        <v>290</v>
-      </c>
-      <c r="I129" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="K129" t="b">
         <v>0</v>
       </c>
       <c r="M129" t="b">
         <v>1</v>
-      </c>
-      <c r="N129" t="b">
-        <v>1</v>
-      </c>
-      <c r="O129" t="b">
-        <v>0</v>
-      </c>
-      <c r="P129" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q129" t="b">
-        <v>0</v>
       </c>
       <c r="R129" t="b">
         <v>0</v>
@@ -7987,7 +7806,7 @@
     </row>
     <row r="130" spans="1:23">
       <c r="A130" t="s">
-        <v>129</v>
+        <v>364</v>
       </c>
       <c r="B130" t="s">
         <v>287</v>
@@ -7998,29 +7817,11 @@
       <c r="D130" t="s">
         <v>313</v>
       </c>
-      <c r="H130" t="s">
-        <v>292</v>
-      </c>
-      <c r="I130" t="s">
-        <v>309</v>
-      </c>
       <c r="K130" t="b">
         <v>0</v>
       </c>
       <c r="M130" t="b">
         <v>1</v>
-      </c>
-      <c r="N130" t="b">
-        <v>0</v>
-      </c>
-      <c r="O130" t="b">
-        <v>0</v>
-      </c>
-      <c r="P130" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q130" t="b">
-        <v>0</v>
       </c>
       <c r="R130" t="b">
         <v>0</v>
@@ -8043,26 +7844,23 @@
     </row>
     <row r="131" spans="1:23">
       <c r="A131" t="s">
-        <v>128</v>
+        <v>296</v>
       </c>
       <c r="B131" t="s">
-        <v>287</v>
+        <v>320</v>
       </c>
       <c r="C131" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D131" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E131" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="H131" t="s">
         <v>292</v>
       </c>
-      <c r="I131" t="s">
-        <v>309</v>
-      </c>
       <c r="K131" t="b">
         <v>0</v>
       </c>
@@ -8070,7 +7868,7 @@
         <v>1</v>
       </c>
       <c r="N131" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O131" t="b">
         <v>0</v>
@@ -8102,7 +7900,7 @@
     </row>
     <row r="132" spans="1:23">
       <c r="A132" t="s">
-        <v>342</v>
+        <v>131</v>
       </c>
       <c r="B132" t="s">
         <v>287</v>
@@ -8114,16 +7912,10 @@
         <v>313</v>
       </c>
       <c r="E132" t="s">
-        <v>481</v>
+        <v>490</v>
       </c>
       <c r="F132" t="s">
-        <v>482</v>
-      </c>
-      <c r="H132" t="s">
-        <v>292</v>
-      </c>
-      <c r="I132" t="s">
-        <v>309</v>
+        <v>491</v>
       </c>
       <c r="K132" t="b">
         <v>0</v>
@@ -8132,7 +7924,7 @@
         <v>1</v>
       </c>
       <c r="N132" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O132" t="b">
         <v>0</v>
@@ -8164,7 +7956,7 @@
     </row>
     <row r="133" spans="1:23">
       <c r="A133" t="s">
-        <v>343</v>
+        <v>130</v>
       </c>
       <c r="B133" t="s">
         <v>287</v>
@@ -8175,11 +7967,17 @@
       <c r="D133" t="s">
         <v>313</v>
       </c>
+      <c r="E133" t="s">
+        <v>347</v>
+      </c>
+      <c r="F133" t="s">
+        <v>491</v>
+      </c>
       <c r="H133" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I133" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K133" t="b">
         <v>0</v>
@@ -8220,22 +8018,25 @@
     </row>
     <row r="134" spans="1:23">
       <c r="A134" t="s">
-        <v>398</v>
+        <v>297</v>
       </c>
       <c r="B134" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C134" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D134" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E134" t="s">
-        <v>475</v>
+        <v>492</v>
       </c>
       <c r="H134" t="s">
-        <v>292</v>
+        <v>290</v>
+      </c>
+      <c r="I134" t="s">
+        <v>308</v>
       </c>
       <c r="K134" t="b">
         <v>0</v>
@@ -8276,23 +8077,23 @@
     </row>
     <row r="135" spans="1:23">
       <c r="A135" t="s">
-        <v>335</v>
+        <v>129</v>
       </c>
       <c r="B135" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C135" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D135" t="s">
-        <v>311</v>
-      </c>
-      <c r="E135" t="s">
-        <v>474</v>
+        <v>313</v>
       </c>
       <c r="H135" t="s">
         <v>292</v>
       </c>
+      <c r="I135" t="s">
+        <v>309</v>
+      </c>
       <c r="K135" t="b">
         <v>0</v>
       </c>
@@ -8300,7 +8101,7 @@
         <v>1</v>
       </c>
       <c r="N135" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O135" t="b">
         <v>0</v>
@@ -8332,22 +8133,25 @@
     </row>
     <row r="136" spans="1:23">
       <c r="A136" t="s">
-        <v>336</v>
+        <v>128</v>
       </c>
       <c r="B136" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C136" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D136" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="E136" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="H136" t="s">
-        <v>290</v>
+        <v>292</v>
+      </c>
+      <c r="I136" t="s">
+        <v>309</v>
       </c>
       <c r="K136" t="b">
         <v>0</v>
@@ -8356,7 +8160,7 @@
         <v>1</v>
       </c>
       <c r="N136" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O136" t="b">
         <v>0</v>
@@ -8387,8 +8191,8 @@
       </c>
     </row>
     <row r="137" spans="1:23">
-      <c r="A137" s="17" t="s">
-        <v>498</v>
+      <c r="A137" t="s">
+        <v>342</v>
       </c>
       <c r="B137" t="s">
         <v>287</v>
@@ -8400,15 +8204,57 @@
         <v>313</v>
       </c>
       <c r="E137" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="F137" t="s">
-        <v>500</v>
+        <v>482</v>
+      </c>
+      <c r="H137" t="s">
+        <v>292</v>
+      </c>
+      <c r="I137" t="s">
+        <v>309</v>
+      </c>
+      <c r="K137" t="b">
+        <v>0</v>
+      </c>
+      <c r="M137" t="b">
+        <v>1</v>
+      </c>
+      <c r="N137" t="b">
+        <v>0</v>
+      </c>
+      <c r="O137" t="b">
+        <v>0</v>
+      </c>
+      <c r="P137" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q137" t="b">
+        <v>0</v>
+      </c>
+      <c r="R137" t="b">
+        <v>0</v>
+      </c>
+      <c r="S137" t="b">
+        <v>0</v>
+      </c>
+      <c r="T137" t="b">
+        <v>0</v>
+      </c>
+      <c r="U137" t="b">
+        <v>0</v>
+      </c>
+      <c r="V137" t="b">
+        <v>0</v>
+      </c>
+      <c r="W137" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:23">
-      <c r="A138" s="17" t="s">
-        <v>501</v>
+      <c r="A138" t="s">
+        <v>343</v>
       </c>
       <c r="B138" t="s">
         <v>287</v>
@@ -8419,42 +8265,120 @@
       <c r="D138" t="s">
         <v>313</v>
       </c>
-      <c r="E138" t="s">
-        <v>503</v>
+      <c r="H138" t="s">
+        <v>292</v>
+      </c>
+      <c r="I138" t="s">
+        <v>309</v>
+      </c>
+      <c r="K138" t="b">
+        <v>0</v>
+      </c>
+      <c r="M138" t="b">
+        <v>1</v>
+      </c>
+      <c r="N138" t="b">
+        <v>1</v>
+      </c>
+      <c r="O138" t="b">
+        <v>0</v>
+      </c>
+      <c r="P138" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q138" t="b">
+        <v>0</v>
+      </c>
+      <c r="R138" t="b">
+        <v>0</v>
+      </c>
+      <c r="S138" t="b">
+        <v>0</v>
+      </c>
+      <c r="T138" t="b">
+        <v>0</v>
+      </c>
+      <c r="U138" t="b">
+        <v>0</v>
+      </c>
+      <c r="V138" t="b">
+        <v>0</v>
+      </c>
+      <c r="W138" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:23">
-      <c r="A139" s="17" t="s">
-        <v>502</v>
+      <c r="A139" t="s">
+        <v>398</v>
       </c>
       <c r="B139" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C139" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D139" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E139" t="s">
-        <v>504</v>
+        <v>475</v>
+      </c>
+      <c r="H139" t="s">
+        <v>292</v>
+      </c>
+      <c r="K139" t="b">
+        <v>0</v>
+      </c>
+      <c r="M139" t="b">
+        <v>1</v>
+      </c>
+      <c r="N139" t="b">
+        <v>1</v>
+      </c>
+      <c r="O139" t="b">
+        <v>0</v>
+      </c>
+      <c r="P139" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q139" t="b">
+        <v>0</v>
+      </c>
+      <c r="R139" t="b">
+        <v>0</v>
+      </c>
+      <c r="S139" t="b">
+        <v>0</v>
+      </c>
+      <c r="T139" t="b">
+        <v>0</v>
+      </c>
+      <c r="U139" t="b">
+        <v>0</v>
+      </c>
+      <c r="V139" t="b">
+        <v>0</v>
+      </c>
+      <c r="W139" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:23">
       <c r="A140" t="s">
-        <v>358</v>
+        <v>335</v>
       </c>
       <c r="B140" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C140" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D140" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E140" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H140" t="s">
         <v>292</v>
@@ -8463,7 +8387,7 @@
         <v>0</v>
       </c>
       <c r="M140" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N140" t="b">
         <v>1</v>
@@ -8498,175 +8422,100 @@
     </row>
     <row r="141" spans="1:23">
       <c r="A141" t="s">
-        <v>359</v>
+        <v>336</v>
       </c>
       <c r="B141" t="s">
+        <v>288</v>
+      </c>
+      <c r="C141" t="s">
+        <v>315</v>
+      </c>
+      <c r="D141" t="s">
+        <v>324</v>
+      </c>
+      <c r="E141" t="s">
+        <v>473</v>
+      </c>
+      <c r="H141" t="s">
+        <v>290</v>
+      </c>
+      <c r="K141" t="b">
+        <v>0</v>
+      </c>
+      <c r="M141" t="b">
+        <v>1</v>
+      </c>
+      <c r="N141" t="b">
+        <v>1</v>
+      </c>
+      <c r="O141" t="b">
+        <v>0</v>
+      </c>
+      <c r="P141" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q141" t="b">
+        <v>0</v>
+      </c>
+      <c r="R141" t="b">
+        <v>0</v>
+      </c>
+      <c r="S141" t="b">
+        <v>0</v>
+      </c>
+      <c r="T141" t="b">
+        <v>0</v>
+      </c>
+      <c r="U141" t="b">
+        <v>0</v>
+      </c>
+      <c r="V141" t="b">
+        <v>0</v>
+      </c>
+      <c r="W141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:23">
+      <c r="A142" s="17" t="s">
+        <v>498</v>
+      </c>
+      <c r="B142" t="s">
         <v>287</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C142" t="s">
         <v>314</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D142" t="s">
         <v>313</v>
       </c>
-      <c r="E141" t="s">
-        <v>477</v>
-      </c>
-      <c r="H141" t="s">
-        <v>292</v>
-      </c>
-      <c r="K141" t="b">
-        <v>0</v>
-      </c>
-      <c r="M141" t="b">
-        <v>0</v>
-      </c>
-      <c r="N141" t="b">
-        <v>1</v>
-      </c>
-      <c r="O141" t="b">
-        <v>0</v>
-      </c>
-      <c r="P141" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q141" t="b">
-        <v>0</v>
-      </c>
-      <c r="R141" t="b">
-        <v>0</v>
-      </c>
-      <c r="S141" t="b">
-        <v>0</v>
-      </c>
-      <c r="T141" t="b">
-        <v>0</v>
-      </c>
-      <c r="U141" t="b">
-        <v>0</v>
-      </c>
-      <c r="V141" t="b">
-        <v>0</v>
-      </c>
-      <c r="W141" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:23">
-      <c r="A142" t="s">
-        <v>357</v>
-      </c>
-      <c r="B142" t="s">
-        <v>288</v>
-      </c>
-      <c r="C142" t="s">
-        <v>319</v>
-      </c>
-      <c r="D142" t="s">
-        <v>312</v>
-      </c>
       <c r="E142" t="s">
-        <v>478</v>
-      </c>
-      <c r="H142" t="s">
-        <v>292</v>
-      </c>
-      <c r="K142" t="b">
-        <v>0</v>
-      </c>
-      <c r="M142" t="b">
-        <v>0</v>
-      </c>
-      <c r="N142" t="b">
-        <v>1</v>
-      </c>
-      <c r="O142" t="b">
-        <v>0</v>
-      </c>
-      <c r="P142" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q142" t="b">
-        <v>0</v>
-      </c>
-      <c r="R142" t="b">
-        <v>0</v>
-      </c>
-      <c r="S142" t="b">
-        <v>0</v>
-      </c>
-      <c r="T142" t="b">
-        <v>0</v>
-      </c>
-      <c r="U142" t="b">
-        <v>0</v>
-      </c>
-      <c r="V142" t="b">
-        <v>0</v>
-      </c>
-      <c r="W142" t="b">
-        <v>0</v>
+        <v>499</v>
+      </c>
+      <c r="F142" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="143" spans="1:23">
-      <c r="A143" t="s">
-        <v>294</v>
+      <c r="A143" s="17" t="s">
+        <v>501</v>
       </c>
       <c r="B143" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C143" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D143" t="s">
-        <v>311</v>
-      </c>
-      <c r="E143" s="9" t="s">
-        <v>479</v>
-      </c>
-      <c r="H143" t="s">
-        <v>292</v>
-      </c>
-      <c r="K143" t="b">
-        <v>0</v>
-      </c>
-      <c r="M143" t="b">
-        <v>1</v>
-      </c>
-      <c r="N143" t="b">
-        <v>1</v>
-      </c>
-      <c r="O143" t="b">
-        <v>1</v>
-      </c>
-      <c r="P143" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q143" t="b">
-        <v>1</v>
-      </c>
-      <c r="R143" t="b">
-        <v>0</v>
-      </c>
-      <c r="S143" t="b">
-        <v>0</v>
-      </c>
-      <c r="T143" t="b">
-        <v>0</v>
-      </c>
-      <c r="U143" t="b">
-        <v>0</v>
-      </c>
-      <c r="V143" t="b">
-        <v>0</v>
-      </c>
-      <c r="W143" t="b">
-        <v>0</v>
+        <v>313</v>
+      </c>
+      <c r="E143" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="144" spans="1:23">
-      <c r="A144" t="s">
-        <v>355</v>
+      <c r="A144" s="17" t="s">
+        <v>502</v>
       </c>
       <c r="B144" t="s">
         <v>287</v>
@@ -8677,63 +8526,26 @@
       <c r="D144" t="s">
         <v>313</v>
       </c>
-      <c r="E144" s="9" t="s">
-        <v>480</v>
-      </c>
-      <c r="H144" t="s">
-        <v>292</v>
-      </c>
-      <c r="K144" t="b">
-        <v>0</v>
-      </c>
-      <c r="M144" t="b">
-        <v>1</v>
-      </c>
-      <c r="N144" t="b">
-        <v>1</v>
-      </c>
-      <c r="O144" t="b">
-        <v>1</v>
-      </c>
-      <c r="P144" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q144" t="b">
-        <v>1</v>
-      </c>
-      <c r="R144" t="b">
-        <v>0</v>
-      </c>
-      <c r="S144" t="b">
-        <v>0</v>
-      </c>
-      <c r="T144" t="b">
-        <v>0</v>
-      </c>
-      <c r="U144" t="b">
-        <v>0</v>
-      </c>
-      <c r="V144" t="b">
-        <v>0</v>
-      </c>
-      <c r="W144" t="b">
-        <v>0</v>
+      <c r="E144" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="145" spans="1:23">
       <c r="A145" t="s">
-        <v>295</v>
+        <v>358</v>
       </c>
       <c r="B145" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C145" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D145" t="s">
-        <v>311</v>
-      </c>
-      <c r="E145" s="3"/>
+        <v>313</v>
+      </c>
+      <c r="E145" t="s">
+        <v>476</v>
+      </c>
       <c r="H145" t="s">
         <v>292</v>
       </c>
@@ -8741,19 +8553,19 @@
         <v>0</v>
       </c>
       <c r="M145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N145" t="b">
         <v>1</v>
       </c>
       <c r="O145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R145" t="b">
         <v>0</v>
@@ -8774,8 +8586,286 @@
         <v>0</v>
       </c>
     </row>
+    <row r="146" spans="1:23">
+      <c r="A146" t="s">
+        <v>359</v>
+      </c>
+      <c r="B146" t="s">
+        <v>287</v>
+      </c>
+      <c r="C146" t="s">
+        <v>314</v>
+      </c>
+      <c r="D146" t="s">
+        <v>313</v>
+      </c>
+      <c r="E146" t="s">
+        <v>477</v>
+      </c>
+      <c r="H146" t="s">
+        <v>292</v>
+      </c>
+      <c r="K146" t="b">
+        <v>0</v>
+      </c>
+      <c r="M146" t="b">
+        <v>0</v>
+      </c>
+      <c r="N146" t="b">
+        <v>1</v>
+      </c>
+      <c r="O146" t="b">
+        <v>0</v>
+      </c>
+      <c r="P146" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q146" t="b">
+        <v>0</v>
+      </c>
+      <c r="R146" t="b">
+        <v>0</v>
+      </c>
+      <c r="S146" t="b">
+        <v>0</v>
+      </c>
+      <c r="T146" t="b">
+        <v>0</v>
+      </c>
+      <c r="U146" t="b">
+        <v>0</v>
+      </c>
+      <c r="V146" t="b">
+        <v>0</v>
+      </c>
+      <c r="W146" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:23">
+      <c r="A147" t="s">
+        <v>357</v>
+      </c>
+      <c r="B147" t="s">
+        <v>288</v>
+      </c>
+      <c r="C147" t="s">
+        <v>319</v>
+      </c>
+      <c r="D147" t="s">
+        <v>312</v>
+      </c>
+      <c r="E147" t="s">
+        <v>478</v>
+      </c>
+      <c r="H147" t="s">
+        <v>292</v>
+      </c>
+      <c r="K147" t="b">
+        <v>0</v>
+      </c>
+      <c r="M147" t="b">
+        <v>0</v>
+      </c>
+      <c r="N147" t="b">
+        <v>1</v>
+      </c>
+      <c r="O147" t="b">
+        <v>0</v>
+      </c>
+      <c r="P147" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q147" t="b">
+        <v>0</v>
+      </c>
+      <c r="R147" t="b">
+        <v>0</v>
+      </c>
+      <c r="S147" t="b">
+        <v>0</v>
+      </c>
+      <c r="T147" t="b">
+        <v>0</v>
+      </c>
+      <c r="U147" t="b">
+        <v>0</v>
+      </c>
+      <c r="V147" t="b">
+        <v>0</v>
+      </c>
+      <c r="W147" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:23">
+      <c r="A148" t="s">
+        <v>294</v>
+      </c>
+      <c r="B148" t="s">
+        <v>289</v>
+      </c>
+      <c r="C148" t="s">
+        <v>318</v>
+      </c>
+      <c r="D148" t="s">
+        <v>311</v>
+      </c>
+      <c r="E148" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="H148" t="s">
+        <v>292</v>
+      </c>
+      <c r="K148" t="b">
+        <v>0</v>
+      </c>
+      <c r="M148" t="b">
+        <v>1</v>
+      </c>
+      <c r="N148" t="b">
+        <v>1</v>
+      </c>
+      <c r="O148" t="b">
+        <v>1</v>
+      </c>
+      <c r="P148" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q148" t="b">
+        <v>1</v>
+      </c>
+      <c r="R148" t="b">
+        <v>0</v>
+      </c>
+      <c r="S148" t="b">
+        <v>0</v>
+      </c>
+      <c r="T148" t="b">
+        <v>0</v>
+      </c>
+      <c r="U148" t="b">
+        <v>0</v>
+      </c>
+      <c r="V148" t="b">
+        <v>0</v>
+      </c>
+      <c r="W148" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:23">
+      <c r="A149" t="s">
+        <v>355</v>
+      </c>
+      <c r="B149" t="s">
+        <v>287</v>
+      </c>
+      <c r="C149" t="s">
+        <v>314</v>
+      </c>
+      <c r="D149" t="s">
+        <v>313</v>
+      </c>
+      <c r="E149" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="H149" t="s">
+        <v>292</v>
+      </c>
+      <c r="K149" t="b">
+        <v>0</v>
+      </c>
+      <c r="M149" t="b">
+        <v>1</v>
+      </c>
+      <c r="N149" t="b">
+        <v>1</v>
+      </c>
+      <c r="O149" t="b">
+        <v>1</v>
+      </c>
+      <c r="P149" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q149" t="b">
+        <v>1</v>
+      </c>
+      <c r="R149" t="b">
+        <v>0</v>
+      </c>
+      <c r="S149" t="b">
+        <v>0</v>
+      </c>
+      <c r="T149" t="b">
+        <v>0</v>
+      </c>
+      <c r="U149" t="b">
+        <v>0</v>
+      </c>
+      <c r="V149" t="b">
+        <v>0</v>
+      </c>
+      <c r="W149" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:23">
+      <c r="A150" t="s">
+        <v>295</v>
+      </c>
+      <c r="B150" t="s">
+        <v>289</v>
+      </c>
+      <c r="C150" t="s">
+        <v>318</v>
+      </c>
+      <c r="D150" t="s">
+        <v>311</v>
+      </c>
+      <c r="E150" s="3"/>
+      <c r="H150" t="s">
+        <v>292</v>
+      </c>
+      <c r="K150" t="b">
+        <v>0</v>
+      </c>
+      <c r="M150" t="b">
+        <v>1</v>
+      </c>
+      <c r="N150" t="b">
+        <v>1</v>
+      </c>
+      <c r="O150" t="b">
+        <v>1</v>
+      </c>
+      <c r="P150" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q150" t="b">
+        <v>1</v>
+      </c>
+      <c r="R150" t="b">
+        <v>0</v>
+      </c>
+      <c r="S150" t="b">
+        <v>0</v>
+      </c>
+      <c r="T150" t="b">
+        <v>0</v>
+      </c>
+      <c r="U150" t="b">
+        <v>0</v>
+      </c>
+      <c r="V150" t="b">
+        <v>0</v>
+      </c>
+      <c r="W150" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:X145" xr:uid="{434BD60A-FB0C-6840-A282-2A366498F430}"/>
+  <autoFilter ref="A1:X150" xr:uid="{434BD60A-FB0C-6840-A282-2A366498F430}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
tape package evolution.  adds more checks and starts PD extention
</commit_message>
<xml_diff>
--- a/DataDictionary05092023.xlsx
+++ b/DataDictionary05092023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crmerrill/lib/tapestratification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B246711-7600-B549-941B-D2B2BF0A78F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C77CB1A-DAE9-D941-A832-9A08F2CC78F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="47500" windowHeight="23940" xr2:uid="{0CFC8428-1E30-8A46-AA94-E08A216C8C38}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="47500" windowHeight="23940" xr2:uid="{0CFC8428-1E30-8A46-AA94-E08A216C8C38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$X$150</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$I$91</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="500"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>